<commit_message>
Test: Additional unit tests for attribute to test built-in attribute limit
</commit_message>
<xml_diff>
--- a/DC20Models.nUnitTests/Unit Tests/BlackBox_Attribute.xlsx
+++ b/DC20Models.nUnitTests/Unit Tests/BlackBox_Attribute.xlsx
@@ -1,21 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Blazor\DC20 Character Sheet\DC20Models\DC20Models.nUnitTests\Unit Tests\Attribute\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Blazor\DC20 Character Sheet\DC20Models\DC20Models.nUnitTests\Unit Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBD1CAAF-8C60-4E72-96FA-B4810E3E9DD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{226D92A6-944A-40D9-8F7B-E44C37C0A524}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{B6E2DC97-E5A5-4906-BB28-0603128A6FF0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B6E2DC97-E5A5-4906-BB28-0603128A6FF0}"/>
   </bookViews>
   <sheets>
     <sheet name="ValueTest" sheetId="1" r:id="rId1"/>
     <sheet name="SaveTest" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ValueTest!$A$1:$I$17</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -37,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="34">
   <si>
     <t>Valid Input</t>
   </si>
@@ -115,6 +118,30 @@
   </si>
   <si>
     <t>greater than limit, max level</t>
+  </si>
+  <si>
+    <t>level/2</t>
+  </si>
+  <si>
+    <t>level</t>
+  </si>
+  <si>
+    <t>minimum level, max legal value</t>
+  </si>
+  <si>
+    <t>level 10 limit increase</t>
+  </si>
+  <si>
+    <t>exceed level 10 limit</t>
+  </si>
+  <si>
+    <t>level 15 limit increase</t>
+  </si>
+  <si>
+    <t>exceed level 15 limit</t>
+  </si>
+  <si>
+    <t>exceed max limit</t>
   </si>
 </sst>
 </file>
@@ -166,7 +193,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -178,6 +205,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -514,301 +553,457 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B072AB2B-2B84-49ED-8A2B-DA516F62DDCB}">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="1"/>
-    <col min="6" max="6" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="23.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.28515625" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4" t="s">
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="J1" s="2"/>
+      <c r="I1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="6"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="3" t="s">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="6"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="7">
+        <v>1</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="7">
+        <v>1</v>
+      </c>
+      <c r="F3" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G3" s="7">
+        <v>1</v>
+      </c>
+      <c r="H3" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="7">
+        <v>2</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="7">
+        <v>-2</v>
+      </c>
+      <c r="F4" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G4" s="7">
+        <v>1</v>
+      </c>
+      <c r="H4" s="7">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
+        <v>3</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="7">
+        <v>-3</v>
+      </c>
+      <c r="F5" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G5" s="7">
+        <v>1</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="7">
+        <v>4</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="7">
+        <v>3</v>
+      </c>
+      <c r="F6" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G6" s="7">
+        <v>1</v>
+      </c>
+      <c r="H6" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="7">
+        <v>4</v>
+      </c>
+      <c r="F7" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G7" s="7">
+        <v>1</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
+        <v>6</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="7">
+        <v>4</v>
+      </c>
+      <c r="F8" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G8" s="7">
+        <v>5</v>
+      </c>
+      <c r="H8" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
+        <v>7</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="7">
+        <v>5</v>
+      </c>
+      <c r="F9" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G9" s="7">
+        <v>5</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="7">
+        <v>8</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="7">
+        <v>7</v>
+      </c>
+      <c r="F10" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G10" s="7">
+        <v>20</v>
+      </c>
+      <c r="H10" s="7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="7">
+        <v>9</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="7">
+        <v>10</v>
+      </c>
+      <c r="F11" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G11" s="7">
+        <v>20</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="7">
+        <v>10</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="7">
+        <v>3</v>
+      </c>
+      <c r="F12" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G12" s="7">
+        <v>1</v>
+      </c>
+      <c r="H12" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="7">
         <v>11</v>
       </c>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="2"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="B13" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="7">
+        <v>5</v>
+      </c>
+      <c r="F13" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G13" s="7">
         <v>10</v>
       </c>
-      <c r="E3" s="1">
-        <v>1</v>
-      </c>
-      <c r="F3" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="G3" s="1">
-        <v>1</v>
-      </c>
-      <c r="H3" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="H13" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="7">
+        <v>12</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="7">
+        <v>6</v>
+      </c>
+      <c r="F14" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G14" s="7">
         <v>10</v>
       </c>
-      <c r="E4" s="1">
-        <v>-2</v>
-      </c>
-      <c r="F4" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="G4" s="1">
-        <v>1</v>
-      </c>
-      <c r="H4" s="1">
-        <v>-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1" t="s">
+      <c r="H14" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="7">
+        <v>13</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" s="7">
+        <v>6</v>
+      </c>
+      <c r="F15" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G15" s="7">
         <v>15</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="H15" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="7">
+        <v>14</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" s="7">
+        <v>7</v>
+      </c>
+      <c r="F16" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G16" s="7">
+        <v>15</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="7">
         <v>16</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="B17" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" s="7">
         <v>10</v>
       </c>
-      <c r="E5" s="1">
-        <v>-3</v>
-      </c>
-      <c r="F5" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="G5" s="1">
-        <v>1</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>4</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" s="1" t="s">
+      <c r="F17" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G17" s="7">
         <v>20</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="1">
-        <v>3</v>
-      </c>
-      <c r="F6" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="G6" s="1">
-        <v>1</v>
-      </c>
-      <c r="H6" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>5</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="1">
-        <v>4</v>
-      </c>
-      <c r="F7" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="G7" s="1">
-        <v>1</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>6</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="1">
-        <v>4</v>
-      </c>
-      <c r="F8" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="G8" s="1">
-        <v>5</v>
-      </c>
-      <c r="H8" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>7</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="1">
-        <v>5</v>
-      </c>
-      <c r="F9" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="G9" s="1">
-        <v>5</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>8</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="1">
-        <v>7</v>
-      </c>
-      <c r="F10" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="G10" s="1">
-        <v>20</v>
-      </c>
-      <c r="H10" s="1">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>9</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" s="1">
-        <v>10</v>
-      </c>
-      <c r="F11" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="G11" s="1">
-        <v>20</v>
-      </c>
-      <c r="H11" s="1" t="s">
+      <c r="H17" s="7" t="s">
         <v>19</v>
       </c>
     </row>
@@ -829,8 +1024,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86460E33-CEEB-4EE7-A91F-B5FF84DB84BE}">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>